<commit_message>
CHANGES:     db changes     questionnaire survey data should be written in db     valid survey check     bugfixes NEXT CHANGES SOON:     little design changes in questionnaire     clearer variable names
</commit_message>
<xml_diff>
--- a/object_rocket.xlsx
+++ b/object_rocket.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -383,160 +383,175 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>FAKE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Feedback_Text</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Form_Type</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Gender</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Like</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Neutral</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Next_Movie_To_Watch</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Pers_01</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_01</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_02</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_03</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_04</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_05</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_06</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_07</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_08</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_09</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_10</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_11</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_12</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_13</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_14</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_15</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_16</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_17</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_18</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Question_Rec_19</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Timestamp_page_1</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_20</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Timestamp_page_2</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Timestamp_page_3</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Timestamp_page_4</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Timestamp_page_submit</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp_start_session</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Watchlist</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>_id</t>
         </is>
@@ -545,52 +560,50 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>5e77cbf7121e4075ebc42456</t>
+          <t>5e7bec2d9984da06eb63fb46</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>66+</t>
+          <t>26-40</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[6, 19, 33]</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>test123</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+          <t>[22, 40]</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>test 6</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>female</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[3, 32, 37]</t>
+          <t>male</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[27, 28, 40]</t>
+          <t>[9, 20, 36]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>[3, 29, 44]</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t xml:space="preserve">The Wolf of Wall Street </t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="K2" t="inlineStr">
         <is>
           <t>1</t>
@@ -598,32 +611,32 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -681,29 +694,44 @@
           <t>1</t>
         </is>
       </c>
-      <c r="AC2" s="2" t="n">
-        <v>43912.85705554398</v>
-      </c>
-      <c r="AD2" s="2" t="n">
-        <v>43912.85723670139</v>
-      </c>
-      <c r="AE2" s="2" t="n">
-        <v>43912.85730805556</v>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="AF2" s="2" t="n">
-        <v>43912.85766184028</v>
+        <v>43915.9866840625</v>
       </c>
       <c r="AG2" s="2" t="n">
-        <v>43912.85767553241</v>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>['The Wolf of Wall Street ', 'The Silence of the Lambs']</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>5e77cbf7121e4075ebc42456</t>
+        <v>43915.98673648148</v>
+      </c>
+      <c r="AH2" s="2" t="n">
+        <v>43915.98717037037</v>
+      </c>
+      <c r="AI2" s="2" t="n">
+        <v>43915.98718770834</v>
+      </c>
+      <c r="AJ2" s="2" t="n">
+        <v>43915.98652409722</v>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>['The Prestige', 'The Wolf of Wall Street ']</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>5e7bec2d9984da06eb63fb46</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CHANGES:     db changes     all questionnaire survey data is written in db     valid survey check     bugfixes
NEXT CHANGES SOON:
    little design changes in questionnaire
    clearer variable names
</commit_message>
<xml_diff>
--- a/object_rocket.xlsx
+++ b/object_rocket.xlsx
@@ -423,149 +423,149 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Question_Rec_01</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_02</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_03</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_04</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_05</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_06</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_07</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_08</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_09</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_10</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_11</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_12</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_13</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_14</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_15</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_16</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_17</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_18</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_19</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Question_Rec_20</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp_page_2</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp_page_3</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp_page_4</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp_page_submit</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp_start_session</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Watchlist</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>_id</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
           <t>Question_Pers_02</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_01</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_02</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_03</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_04</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_05</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_06</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_07</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_08</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_09</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_10</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_11</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_12</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_13</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_14</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_15</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_16</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_17</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_18</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_19</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Question_Rec_20</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>Timestamp_page_2</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Timestamp_page_3</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>Timestamp_page_4</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>Timestamp_page_submit</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Timestamp_start_session</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>Watchlist</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>_id</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>5e7c726a5391510f178d27f7</t>
+          <t>5e7c7b2cafa356110ffc234d</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -575,202 +575,194 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[3, 25, 31, 32]</t>
+          <t>[1, 6, 7, 8, 9, 10, 11, 14, 17, 18, 19, 21, 22, 23, 25, 26, 27, 32, 33, 34, 35, 37, 38, 39, 41, 43, 44, 45, 46, 48]</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>male</t>
+          <t>female</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[12, 14]</t>
+          <t>[13, 29, 31, 36, 40]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[26, 38, 45]</t>
+          <t>[2, 3, 4, 15, 16, 20, 24, 28, 47]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>The Silence of the Lambs</t>
+          <t>Interstellar</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="AF2" s="2" t="n">
+        <v>43916.41025799768</v>
       </c>
       <c r="AG2" s="2" t="n">
-        <v>43916.38441706019</v>
+        <v>43916.41052859954</v>
       </c>
       <c r="AH2" s="2" t="n">
-        <v>43916.38446512732</v>
+        <v>43916.41087674769</v>
       </c>
       <c r="AI2" s="2" t="n">
-        <v>43916.38492199074</v>
+        <v>43916.41088719908</v>
       </c>
       <c r="AJ2" s="2" t="n">
-        <v>43916.38493159723</v>
-      </c>
-      <c r="AK2" s="2" t="n">
-        <v>43916.38427173611</v>
+        <v>43916.40973605324</v>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>['Terminator 2: Judgment Day', 'Up', 'Shutter Island', 'The Wolf of Wall Street ', 'Batman Begins', 'Interstellar', 'The Prestige', 'The Silence of the Lambs', 'Django Unchained']</t>
+        </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>['The Silence of the Lambs', 'Up']</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>5e7c726a5391510f178d27f7</t>
-        </is>
-      </c>
+          <t>5e7c7b2cafa356110ffc234d</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>5e7c72fbc312c289435c47b6</t>
+          <t>5e7c7b9aafa356110ffc234e</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>41-65</t>
+          <t>19-25</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[20, 21]</t>
+          <t>[16, 17, 27]</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>test xy</t>
+          <t>Test besser!</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -779,25 +771,29 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>[4, 16, 17]</t>
+          <t>[3, 5, 18, 24, 26, 31, 37]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>[1, 5, 40]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Interstellar</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>1</t>
@@ -890,49 +886,49 @@
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AF3" s="2" t="n">
+        <v>43916.41112211806</v>
       </c>
       <c r="AG3" s="2" t="n">
-        <v>43916.38613790509</v>
+        <v>43916.41116734954</v>
       </c>
       <c r="AH3" s="2" t="n">
-        <v>43916.38620767361</v>
+        <v>43916.41213149305</v>
       </c>
       <c r="AI3" s="2" t="n">
-        <v>43916.38659841435</v>
+        <v>43916.41215311342</v>
       </c>
       <c r="AJ3" s="2" t="n">
-        <v>43916.38660892361</v>
-      </c>
-      <c r="AK3" s="2" t="n">
-        <v>43916.38596059028</v>
+        <v>43916.41098200231</v>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>['Interstellar', 'Up']</t>
+        </is>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>['Shutter Island', 'Interstellar', 'Terminator 2: Judgment Day']</t>
+          <t>5e7c7b9aafa356110ffc234e</t>
         </is>
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>5e7c72fbc312c289435c47b6</t>
+          <t>7</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>5e7c797a232a8c322396ea25</t>
+          <t>5e7c7d5666279b29e2ae6a0c</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>19-25</t>
+          <t>66+</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -941,167 +937,163 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>2</v>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>female</t>
+          <t>male</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[1, 3, 6, 16, 24, 28, 35, 41, 42]</t>
+          <t>[17, 32, 34]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[2, 5, 8, 10, 26, 29, 34, 36]</t>
+          <t>[1, 5, 35, 43]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Interstellar</t>
+          <t xml:space="preserve">The Wolf of Wall Street </t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
+      <c r="AF4" s="2" t="n">
+        <v>43916.4167841551</v>
       </c>
       <c r="AG4" s="2" t="n">
-        <v>43916.40555707176</v>
+        <v>43916.41687724537</v>
       </c>
       <c r="AH4" s="2" t="n">
-        <v>43916.40564560185</v>
+        <v>43916.41729181713</v>
       </c>
       <c r="AI4" s="2" t="n">
-        <v>43916.4058502199</v>
+        <v>43916.41730074074</v>
       </c>
       <c r="AJ4" s="2" t="n">
-        <v>43916.40586050926</v>
-      </c>
-      <c r="AK4" s="2" t="n">
-        <v>43916.4052921412</v>
+        <v>43916.41659936342</v>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>['The Wolf of Wall Street ', 'The Prestige', 'Shutter Island']</t>
+        </is>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>['Terminator 2: Judgment Day', 'Interstellar']</t>
-        </is>
-      </c>
-      <c r="AM4" t="inlineStr">
-        <is>
-          <t>5e7c797a232a8c322396ea25</t>
-        </is>
-      </c>
+          <t>5e7c7d5666279b29e2ae6a0c</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>